<commit_message>
Increasingly difficult to find median income information once I reach about 1940.
</commit_message>
<xml_diff>
--- a/prelim_data.xlsx
+++ b/prelim_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="34400" windowHeight="23260" tabRatio="500"/>
+    <workbookView xWindow="19900" yWindow="-80" windowWidth="19080" windowHeight="23240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,23 +18,168 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+  <si>
+    <t>US Census: Current Population Reports Consumer Income 1945</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prologue Magazine, Spring 2012, Vol 44, No 1: Brother, Can You Spare a Dime?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>* Value is given as mean income per family</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1935 *</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>100 Years of Consumer Spending, 1934-1936, US Bureau of Labor Statistics</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>All values in the Median Household Income column indicate value unadjusted for inflation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census: Money Income of Households, Families, and Persons in the United States, 1990</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census: Money Income of Households, Families, and Persons in the United States, 1985</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census: Money Income of Households, Families, and Persons in the United States, 1980</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census: Household Money Income in 1975 and Selected Social and Economic Characteristics of Households</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census: Current Population Reports Consumer Income 1970</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>When possible, figures come from the US Census P60 series of reports</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census: Current Population Reports Consumer Income 1965</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census: Current Population Reports Consumer Income 1960</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016 VALUE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US INCOME 1900 TO PRESENT (2016)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>YEAR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>INFLATION %</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOURCE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOTES:</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2014 is the most recent year with census data available</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census, Income &amp; Poverty in the United States Sept. 2015 report</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEDIAN HOUSEHOLD INCOME</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census: Income, Poverty, &amp; Health Insurance Coverage, 2010</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census: Income, Poverty, &amp; Health Insurance Coverage, 2005</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census: Money Income in the United States 2000</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census: Money Income in the United States 1995</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color indexed="9"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="9"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="62"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -42,14 +187,125 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -378,14 +634,374 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
-  <sheetData/>
-  <sheetCalcPr fullCalcOnLoad="1"/>
+  <cols>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="19" thickBot="1">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:5" ht="27" thickBot="1">
+      <c r="A2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>1900</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>1905</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>1910</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>1915</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1">
+        <v>1920</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1">
+        <v>1925</v>
+      </c>
+      <c r="B8" s="7">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>1930</v>
+      </c>
+      <c r="B9" s="7">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:5" ht="39">
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="7">
+        <v>1524</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="39">
+      <c r="A11" s="1">
+        <v>1940</v>
+      </c>
+      <c r="B11" s="7">
+        <v>1368</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="26">
+      <c r="A12" s="1">
+        <v>1945</v>
+      </c>
+      <c r="B12" s="7">
+        <v>2379</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="26">
+      <c r="A13" s="1">
+        <v>1950</v>
+      </c>
+      <c r="B13" s="7">
+        <v>3319</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="26">
+      <c r="A14" s="1">
+        <v>1955</v>
+      </c>
+      <c r="B14" s="7">
+        <v>4421</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="26">
+      <c r="A15" s="1">
+        <v>1960</v>
+      </c>
+      <c r="B15" s="7">
+        <v>5620</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="26">
+      <c r="A16" s="1">
+        <v>1965</v>
+      </c>
+      <c r="B16" s="7">
+        <v>6882</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="26">
+      <c r="A17" s="1">
+        <v>1970</v>
+      </c>
+      <c r="B17" s="7">
+        <v>8730</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="52">
+      <c r="A18" s="1">
+        <v>1975</v>
+      </c>
+      <c r="B18" s="7">
+        <v>11800</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="39">
+      <c r="A19" s="1">
+        <v>1980</v>
+      </c>
+      <c r="B19" s="7">
+        <v>17710</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="39">
+      <c r="A20" s="1">
+        <v>1985</v>
+      </c>
+      <c r="B20" s="7">
+        <v>23620</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="39">
+      <c r="A21" s="1">
+        <v>1990</v>
+      </c>
+      <c r="B21" s="7">
+        <v>29943</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="26">
+      <c r="A22" s="1">
+        <v>1995</v>
+      </c>
+      <c r="B22" s="7">
+        <v>34076</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="26">
+      <c r="A23" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B23" s="7">
+        <v>42148</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="26">
+      <c r="A24" s="1">
+        <v>2005</v>
+      </c>
+      <c r="B24" s="7">
+        <v>46326</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="26">
+      <c r="A25" s="1">
+        <v>2010</v>
+      </c>
+      <c r="B25" s="7">
+        <v>49445</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="40" thickBot="1">
+      <c r="A26" s="2">
+        <v>2014</v>
+      </c>
+      <c r="B26" s="8">
+        <v>53657</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Completed gathering info for country median incomes. Unable to find data for UAE or Ethiopia
</commit_message>
<xml_diff>
--- a/prelim_data.xlsx
+++ b/prelim_data.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="17680" yWindow="-80" windowWidth="20660" windowHeight="23320" tabRatio="500"/>
+    <workbookView xWindow="24700" yWindow="-80" windowWidth="13520" windowHeight="23320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="130404" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,325 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="108">
+  <si>
+    <t>Bulgaria</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Germany</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>France</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Italy</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spain</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poland</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Netherlands</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Belgium</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Greece</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Portugal</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hungary</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sweden</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Austria</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Switzerland</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.gallup.com/poll/166211/worldwide-median-household-income-000.aspx</t>
+  </si>
+  <si>
+    <t>http://www.gallup.com/poll/166211/worldwide-median-household-income-000.aspx</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Asia</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://stats.oecd.org/Index.aspx?DataSetCode=IDD</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>North America</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>North America</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brazil</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Colombia</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Argentina</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Peru</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Venzuela</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>South America</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>South America</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>South America</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>South America</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Africa</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nigeria</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Egypt</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR of the Congo</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>South Africa</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tanzania</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kenya</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Algeria</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sudan</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Uganda</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Australia</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>New Zealand</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oceania</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oceania</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Country</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Continent</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Source</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Median Household Income (USD)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ukraine</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Romania</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Serbia</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Denmark</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finland</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Norway</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ireland</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Croatia</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Iceland</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>China</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>India</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Europe</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Europe</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Indonesia</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pakistan</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Japan</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>South Korea</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Iran</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Iraq</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Saudi Arabia</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Syria</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vietnam</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kazakhstan</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Asia</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Canada</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEDIAN INCOMES AROUND THE WORLD</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
   <si>
     <t>Inflation-adjusted values calculated via the Bureau of Labor Statistics CPI Calculator: http://data.bls.gov/cgi-bin/cpicalc.pl</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -140,7 +459,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -169,8 +488,14 @@
       <color indexed="9"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="9"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,6 +505,48 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="62"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="18"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="41"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="47"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="45"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="43"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="46"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -327,7 +694,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -347,15 +714,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -385,6 +743,87 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="9" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="8" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="8" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -720,55 +1159,55 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="150" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="18"/>
-    <col min="2" max="2" width="18.28515625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="18" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" style="18" customWidth="1"/>
-    <col min="6" max="16384" width="10.7109375" style="18"/>
+    <col min="1" max="1" width="10.7109375" style="15"/>
+    <col min="2" max="2" width="18.28515625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" style="15" customWidth="1"/>
+    <col min="6" max="16384" width="10.7109375" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19" thickBot="1">
-      <c r="A1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="9"/>
+      <c r="A1" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:5" ht="27" thickBot="1">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>97</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>23</v>
+        <v>103</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>1900</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="10">
         <v>0</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="14">
+      <c r="C3" s="12"/>
+      <c r="D3" s="11">
         <v>0</v>
       </c>
       <c r="E3" s="4"/>
@@ -777,11 +1216,11 @@
       <c r="A4" s="1">
         <v>1905</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="10">
         <v>0</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="14">
+      <c r="D4" s="11">
         <v>0</v>
       </c>
       <c r="E4" s="4"/>
@@ -790,11 +1229,11 @@
       <c r="A5" s="1">
         <v>1910</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="10">
         <v>0</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="14">
+      <c r="D5" s="11">
         <v>0</v>
       </c>
       <c r="E5" s="4"/>
@@ -803,11 +1242,11 @@
       <c r="A6" s="1">
         <v>1915</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="10">
         <v>0</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="14">
+      <c r="D6" s="11">
         <v>0</v>
       </c>
       <c r="E6" s="4"/>
@@ -816,11 +1255,11 @@
       <c r="A7" s="1">
         <v>1920</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="10">
         <v>0</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="14">
+      <c r="D7" s="11">
         <v>0</v>
       </c>
       <c r="E7" s="4"/>
@@ -829,11 +1268,11 @@
       <c r="A8" s="1">
         <v>1925</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="10">
         <v>0</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="14">
+      <c r="D8" s="11">
         <v>0</v>
       </c>
       <c r="E8" s="4"/>
@@ -842,351 +1281,351 @@
       <c r="A9" s="1">
         <v>1930</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="10">
         <v>0</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="14">
+      <c r="D9" s="11">
         <v>0</v>
       </c>
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" ht="39">
       <c r="A10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="13">
+        <v>86</v>
+      </c>
+      <c r="B10" s="10">
         <v>1524</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="7">
         <f>(D10-B10)/B10</f>
         <v>16.299868766404199</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="11">
         <v>26365</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>7</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="39">
       <c r="A11" s="1">
         <v>1940</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="10">
         <v>1368</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="7">
         <f t="shared" ref="C11:C26" si="0">(D11-B11)/B11</f>
         <v>15.929093567251462</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="11">
         <v>23159</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>4</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="26">
       <c r="A12" s="1">
         <v>1945</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="10">
         <v>2379</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="7">
         <f t="shared" si="0"/>
         <v>12.167297183690627</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="11">
         <v>31325</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="26">
       <c r="A13" s="1">
         <v>1950</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="10">
         <v>3319</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="7">
         <f t="shared" si="0"/>
         <v>8.8345887315456455</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="11">
         <v>32641</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>16</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="26">
       <c r="A14" s="1">
         <v>1955</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="10">
         <v>4421</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="7">
         <f t="shared" si="0"/>
         <v>7.8437005202442887</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="11">
         <v>39098</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="26">
       <c r="A15" s="1">
         <v>1960</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="10">
         <v>5620</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="7">
         <f t="shared" si="0"/>
         <v>7.0072953736654808</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="11">
         <v>45001</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="26">
       <c r="A16" s="1">
         <v>1965</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="10">
         <v>6882</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="7">
         <f t="shared" si="0"/>
         <v>6.5242662016855562</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="11">
         <v>51782</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="26">
       <c r="A17" s="1">
         <v>1970</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17" s="10">
         <v>8730</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="7">
         <f t="shared" si="0"/>
         <v>5.1085910652920958</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="11">
         <v>53328</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="52">
       <c r="A18" s="1">
         <v>1975</v>
       </c>
-      <c r="B18" s="13">
+      <c r="B18" s="10">
         <v>11800</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="7">
         <f t="shared" si="0"/>
         <v>3.4055084745762714</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="11">
         <v>51985</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>12</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="39">
       <c r="A19" s="1">
         <v>1980</v>
       </c>
-      <c r="B19" s="13">
+      <c r="B19" s="10">
         <v>17710</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="7">
         <f t="shared" si="0"/>
         <v>1.8763975155279504</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="11">
         <v>50941</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="39">
       <c r="A20" s="1">
         <v>1985</v>
       </c>
-      <c r="B20" s="13">
+      <c r="B20" s="10">
         <v>23620</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="7">
         <f t="shared" si="0"/>
         <v>1.2027519051651143</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="11">
         <v>52029</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="39">
       <c r="A21" s="1">
         <v>1990</v>
       </c>
-      <c r="B21" s="13">
+      <c r="B21" s="10">
         <v>29943</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="7">
         <f t="shared" si="0"/>
         <v>0.81341214975119391</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="11">
         <v>54299</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>9</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="26">
       <c r="A22" s="1">
         <v>1995</v>
       </c>
-      <c r="B22" s="13">
+      <c r="B22" s="10">
         <v>34076</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="7">
         <f t="shared" si="0"/>
         <v>0.555229487028994</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="11">
         <v>52996</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="26">
       <c r="A23" s="1">
         <v>2000</v>
       </c>
-      <c r="B23" s="13">
+      <c r="B23" s="10">
         <v>42148</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="7">
         <f t="shared" si="0"/>
         <v>0.37638796621429249</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="11">
         <v>58012</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="26">
       <c r="A24" s="1">
         <v>2005</v>
       </c>
-      <c r="B24" s="13">
+      <c r="B24" s="10">
         <v>46326</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="7">
         <f t="shared" si="0"/>
         <v>0.21359495747528387</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D24" s="11">
         <v>56221</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="26">
       <c r="A25" s="1">
         <v>2010</v>
       </c>
-      <c r="B25" s="13">
+      <c r="B25" s="10">
         <v>49445</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="7">
         <f t="shared" si="0"/>
         <v>8.6945090504601072E-2</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="11">
         <v>53744</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="40" thickBot="1">
       <c r="A26" s="2">
         <v>2014</v>
       </c>
-      <c r="B26" s="11">
+      <c r="B26" s="8">
         <v>53657</v>
       </c>
-      <c r="C26" s="16">
+      <c r="C26" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="9">
         <v>53657</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>21</v>
+      <c r="A27" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="17"/>
-      <c r="B28" s="17" t="s">
-        <v>5</v>
+      <c r="A28" s="14"/>
+      <c r="B28" s="14" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17" t="s">
-        <v>8</v>
+      <c r="A29" s="14"/>
+      <c r="B29" s="14" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17" t="s">
-        <v>14</v>
+      <c r="A30" s="14"/>
+      <c r="B30" s="14" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17" t="s">
-        <v>0</v>
+      <c r="A31" s="14"/>
+      <c r="B31" s="14" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1201,4 +1640,883 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:D62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="4" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="19" thickBot="1">
+      <c r="A1" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="24"/>
+    </row>
+    <row r="2" spans="1:4" ht="33" thickBot="1">
+      <c r="A2" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="27">
+        <v>33333</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="29">
+        <v>31112</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="29">
+        <v>31617</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="29">
+        <v>20085</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="29">
+        <v>21959</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="29">
+        <v>11074</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="29">
+        <v>15338</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="29">
+        <v>7322</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="29">
+        <v>38584</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="29">
+        <v>26703</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="29">
+        <v>17777</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="29">
+        <v>22913</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="29">
+        <v>16186</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="29">
+        <v>12445</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="29">
+        <v>50514</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="29">
+        <v>34911</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="29">
+        <v>35083</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="29">
+        <v>8487</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="29">
+        <v>8921</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="29">
+        <v>44360</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="29">
+        <v>34615</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="29">
+        <v>51489</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="29">
+        <v>25085</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="29">
+        <v>16231</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="29">
+        <v>27029</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="31">
+        <v>6180</v>
+      </c>
+      <c r="D28" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="31">
+        <v>3168</v>
+      </c>
+      <c r="D29" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="31">
+        <v>2199</v>
+      </c>
+      <c r="D30" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="31">
+        <v>4060</v>
+      </c>
+      <c r="D31" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="31">
+        <v>2819</v>
+      </c>
+      <c r="D32" s="31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="31">
+        <v>33822</v>
+      </c>
+      <c r="D33" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" s="31">
+        <v>40861</v>
+      </c>
+      <c r="D34" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" s="31">
+        <v>12046</v>
+      </c>
+      <c r="D35" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" s="31">
+        <v>4917</v>
+      </c>
+      <c r="D36" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="31">
+        <v>4121</v>
+      </c>
+      <c r="D37" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" s="31">
+        <v>24980</v>
+      </c>
+      <c r="D38" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="31">
+        <v>8193</v>
+      </c>
+      <c r="D39" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="31">
+        <v>0</v>
+      </c>
+      <c r="D40" s="31"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="31">
+        <v>4783</v>
+      </c>
+      <c r="D41" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" s="31">
+        <v>7492</v>
+      </c>
+      <c r="D42" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="33">
+        <v>41280</v>
+      </c>
+      <c r="D43" s="33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="33">
+        <v>11680</v>
+      </c>
+      <c r="D44" s="33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45" s="35">
+        <v>7522</v>
+      </c>
+      <c r="D45" s="35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="35">
+        <v>6544</v>
+      </c>
+      <c r="D46" s="35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="35">
+        <v>14432</v>
+      </c>
+      <c r="D47" s="35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" s="35">
+        <v>5161</v>
+      </c>
+      <c r="D48" s="35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C49" s="35">
+        <v>11239</v>
+      </c>
+      <c r="D49" s="35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B50" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50" s="37">
+        <v>2667</v>
+      </c>
+      <c r="D50" s="37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B51" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C51" s="37">
+        <v>0</v>
+      </c>
+      <c r="D51" s="37"/>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C52" s="37">
+        <v>3111</v>
+      </c>
+      <c r="D52" s="37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B53" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C53" s="37">
+        <v>1988</v>
+      </c>
+      <c r="D53" s="37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B54" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C54" s="37">
+        <v>5217</v>
+      </c>
+      <c r="D54" s="37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B55" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C55" s="37">
+        <v>2154</v>
+      </c>
+      <c r="D55" s="37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B56" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C56" s="37">
+        <v>1870</v>
+      </c>
+      <c r="D56" s="37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B57" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C57" s="37">
+        <v>7849</v>
+      </c>
+      <c r="D57" s="37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B58" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C58" s="37">
+        <v>3640</v>
+      </c>
+      <c r="D58" s="37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="B59" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C59" s="37">
+        <v>1775</v>
+      </c>
+      <c r="D59" s="37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B60" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="C60" s="39">
+        <v>46555</v>
+      </c>
+      <c r="D60" s="39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="14" thickBot="1">
+      <c r="A61" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="B61" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C61" s="41">
+        <v>35562</v>
+      </c>
+      <c r="D61" s="41" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="42"/>
+      <c r="B62" s="43"/>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed JSON files for US historical income tax rates, US historical median incomes, and global median incomes
</commit_message>
<xml_diff>
--- a/prelim_data.xlsx
+++ b/prelim_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="24700" yWindow="-80" windowWidth="13520" windowHeight="23320" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2680" yWindow="-80" windowWidth="13520" windowHeight="23320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,131 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="109">
+  <si>
+    <t>Venezuela</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEDIAN INCOMES AROUND THE WORLD</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inflation-adjusted values calculated via the Bureau of Labor Statistics CPI Calculator: http://data.bls.gov/cgi-bin/cpicalc.pl</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2015 VALUE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>US INCOME 1900 TO PRESENT</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census: Current Population Reports Consumer Income 1945</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prologue Magazine, Spring 2012, Vol 44, No 1: Brother, Can You Spare a Dime?</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>* Value is given as mean income per family</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1935 *</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>100 Years of Consumer Spending, 1934-1936, US Bureau of Labor Statistics</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>All values in the Median Household Income column indicate value unadjusted for inflation</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census: Money Income of Households, Families, and Persons in the United States, 1990</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census: Money Income of Households, Families, and Persons in the United States, 1985</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census: Money Income of Households, Families, and Persons in the United States, 1980</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census: Household Money Income in 1975 and Selected Social and Economic Characteristics of Households</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census: Current Population Reports Consumer Income 1970</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>When possible, figures come from the US Census P60 series of reports</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census: Current Population Reports Consumer Income 1965</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census: Current Population Reports Consumer Income 1960</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>YEAR</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>INFLATION %</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SOURCE</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOTES:</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2014 is the most recent year with census data available</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census, Income &amp; Poverty in the United States Sept. 2015 report</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEDIAN HOUSEHOLD INCOME</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census: Income, Poverty, &amp; Health Insurance Coverage, 2010</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census: Income, Poverty, &amp; Health Insurance Coverage, 2005</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census: Money Income in the United States 2000</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Census: Money Income in the United States 1995</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://stats.oecd.org/Index.aspx?DataSetCode=IDD</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
   <si>
     <t>Bulgaria</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -128,10 +252,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Venzuela</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>South America</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -333,122 +453,6 @@
   </si>
   <si>
     <t>Canada</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>MEDIAN INCOMES AROUND THE WORLD</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Inflation-adjusted values calculated via the Bureau of Labor Statistics CPI Calculator: http://data.bls.gov/cgi-bin/cpicalc.pl</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2015 VALUE</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>US INCOME 1900 TO PRESENT</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>US Census: Current Population Reports Consumer Income 1945</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prologue Magazine, Spring 2012, Vol 44, No 1: Brother, Can You Spare a Dime?</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>* Value is given as mean income per family</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1935 *</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>100 Years of Consumer Spending, 1934-1936, US Bureau of Labor Statistics</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>All values in the Median Household Income column indicate value unadjusted for inflation</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>US Census: Money Income of Households, Families, and Persons in the United States, 1990</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>US Census: Money Income of Households, Families, and Persons in the United States, 1985</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>US Census: Money Income of Households, Families, and Persons in the United States, 1980</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>US Census: Household Money Income in 1975 and Selected Social and Economic Characteristics of Households</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>US Census: Current Population Reports Consumer Income 1970</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>When possible, figures come from the US Census P60 series of reports</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>US Census: Current Population Reports Consumer Income 1965</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>US Census: Current Population Reports Consumer Income 1960</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>YEAR</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>INFLATION %</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SOURCE</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>NOTES:</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2014 is the most recent year with census data available</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>US Census, Income &amp; Poverty in the United States Sept. 2015 report</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>MEDIAN HOUSEHOLD INCOME</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>US Census: Income, Poverty, &amp; Health Insurance Coverage, 2010</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>US Census: Income, Poverty, &amp; Health Insurance Coverage, 2005</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>US Census: Money Income in the United States 2000</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>US Census: Money Income in the United States 1995</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -456,8 +460,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -744,30 +751,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -824,6 +813,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1159,8 +1166,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1174,29 +1181,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19" thickBot="1">
-      <c r="A1" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19"/>
+      <c r="A1" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5" ht="27" thickBot="1">
       <c r="A2" s="3" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>103</v>
+        <v>25</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>98</v>
+        <v>20</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>81</v>
+        <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1292,7 +1299,7 @@
     </row>
     <row r="10" spans="1:5" ht="39">
       <c r="A10" s="1" t="s">
-        <v>86</v>
+        <v>8</v>
       </c>
       <c r="B10" s="10">
         <v>1524</v>
@@ -1305,7 +1312,7 @@
         <v>26365</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>87</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="39">
@@ -1323,7 +1330,7 @@
         <v>23159</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>84</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="26">
@@ -1341,7 +1348,7 @@
         <v>31325</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="26">
@@ -1359,7 +1366,7 @@
         <v>32641</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>96</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="26">
@@ -1377,7 +1384,7 @@
         <v>39098</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>95</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="26">
@@ -1395,7 +1402,7 @@
         <v>45001</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>95</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="26">
@@ -1413,7 +1420,7 @@
         <v>51782</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>95</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="26">
@@ -1431,7 +1438,7 @@
         <v>53328</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>93</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="52">
@@ -1449,7 +1456,7 @@
         <v>51985</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="39">
@@ -1467,7 +1474,7 @@
         <v>50941</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>91</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="39">
@@ -1485,7 +1492,7 @@
         <v>52029</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>90</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="39">
@@ -1503,7 +1510,7 @@
         <v>54299</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>89</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="26">
@@ -1521,7 +1528,7 @@
         <v>52996</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>107</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="26">
@@ -1539,7 +1546,7 @@
         <v>58012</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>106</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="26">
@@ -1557,7 +1564,7 @@
         <v>56221</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>105</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="26">
@@ -1575,7 +1582,7 @@
         <v>53744</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>104</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="40" thickBot="1">
@@ -1593,39 +1600,39 @@
         <v>53657</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>102</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="16" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>101</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="14"/>
       <c r="B28" s="14" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="14"/>
       <c r="B29" s="14" t="s">
-        <v>88</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="14"/>
       <c r="B30" s="14" t="s">
-        <v>94</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="14"/>
       <c r="B31" s="14" t="s">
-        <v>80</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1634,6 +1641,7 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1647,8 +1655,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="200" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1659,860 +1667,860 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="19" thickBot="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="43"/>
+    </row>
+    <row r="2" spans="1:4" ht="33" thickBot="1">
+      <c r="A2" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="24"/>
-    </row>
-    <row r="2" spans="1:4" ht="33" thickBot="1">
-      <c r="A2" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="22" t="s">
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="21">
+        <v>33333</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="23">
+        <v>31112</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="23">
+        <v>31617</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="23">
+        <v>20085</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="23">
+        <v>21959</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="23">
+        <v>11074</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="23">
+        <v>15338</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="23">
+        <v>7322</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="23">
+        <v>38584</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="23">
+        <v>26703</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="23">
+        <v>17777</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="23">
+        <v>22913</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="23">
+        <v>16186</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="23">
+        <v>12445</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="23">
+        <v>50514</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="23">
+        <v>34911</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="23">
+        <v>35083</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="23">
+        <v>8487</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="23">
+        <v>8921</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="23">
+        <v>44360</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" s="23">
+        <v>34615</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="23">
+        <v>51489</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="23">
+        <v>25085</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="23">
+        <v>16231</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="23">
+        <v>27029</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="25">
+        <v>6180</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" s="25">
+        <v>3168</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="25">
+        <v>2199</v>
+      </c>
+      <c r="D30" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="25">
+        <v>4060</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32" s="25">
+        <v>2819</v>
+      </c>
+      <c r="D32" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="25" t="s">
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="25">
+        <v>33822</v>
+      </c>
+      <c r="D33" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="B34" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" s="25">
+        <v>40861</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" s="25">
+        <v>12046</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" s="25">
+        <v>4917</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B37" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="25">
+        <v>4121</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="B38" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" s="25">
+        <v>24980</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C39" s="25">
+        <v>8193</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B40" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="25">
+        <v>0</v>
+      </c>
+      <c r="D40" s="25"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="B41" s="24" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="26" t="s">
+      <c r="C41" s="25">
+        <v>4783</v>
+      </c>
+      <c r="D41" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="B42" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C42" s="25">
+        <v>7492</v>
+      </c>
+      <c r="D42" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="27">
+        <v>41280</v>
+      </c>
+      <c r="D43" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" s="27">
+        <v>11680</v>
+      </c>
+      <c r="D44" s="27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C45" s="29">
+        <v>7522</v>
+      </c>
+      <c r="D45" s="29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" s="29">
+        <v>6544</v>
+      </c>
+      <c r="D46" s="29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" s="29">
+        <v>14432</v>
+      </c>
+      <c r="D47" s="29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B48" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C48" s="29">
+        <v>5161</v>
+      </c>
+      <c r="D48" s="29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49" s="29">
+        <v>11239</v>
+      </c>
+      <c r="D49" s="29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="27">
-        <v>33333</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="29">
-        <v>31112</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="28" t="s">
+      <c r="C50" s="31">
+        <v>2667</v>
+      </c>
+      <c r="D50" s="31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B51" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="29">
-        <v>31617</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="29">
-        <v>20085</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="28" t="s">
+      <c r="C51" s="31">
+        <v>0</v>
+      </c>
+      <c r="D51" s="31"/>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="29">
-        <v>21959</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="29">
-        <v>11074</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="28" t="s">
+      <c r="C52" s="31">
+        <v>3111</v>
+      </c>
+      <c r="D52" s="31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="29">
-        <v>15338</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="29">
-        <v>7322</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="28" t="s">
+      <c r="C53" s="31">
+        <v>1988</v>
+      </c>
+      <c r="D53" s="31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="29">
-        <v>38584</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="29">
-        <v>26703</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="28" t="s">
+      <c r="C54" s="31">
+        <v>5217</v>
+      </c>
+      <c r="D54" s="31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="29">
-        <v>17777</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="29">
-        <v>22913</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="28" t="s">
+      <c r="C55" s="31">
+        <v>2154</v>
+      </c>
+      <c r="D55" s="31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B56" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="29">
-        <v>16186</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="29">
-        <v>12445</v>
-      </c>
-      <c r="D16" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="28" t="s">
+      <c r="C56" s="31">
+        <v>1870</v>
+      </c>
+      <c r="D56" s="31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B57" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="29">
-        <v>50514</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="29">
-        <v>34911</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="28" t="s">
+      <c r="C57" s="31">
+        <v>7849</v>
+      </c>
+      <c r="D57" s="31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B58" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="29">
-        <v>35083</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="29">
-        <v>8487</v>
-      </c>
-      <c r="D20" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="28" t="s">
+      <c r="C58" s="31">
+        <v>3640</v>
+      </c>
+      <c r="D58" s="31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B59" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="29">
-        <v>8921</v>
-      </c>
-      <c r="D21" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="29">
-        <v>44360</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="29">
-        <v>34615</v>
-      </c>
-      <c r="D23" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="29">
-        <v>51489</v>
-      </c>
-      <c r="D24" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="B25" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="29">
-        <v>25085</v>
-      </c>
-      <c r="D25" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="29">
-        <v>16231</v>
-      </c>
-      <c r="D26" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" s="29">
-        <v>27029</v>
-      </c>
-      <c r="D27" s="29" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="C28" s="31">
-        <v>6180</v>
-      </c>
-      <c r="D28" s="31" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" s="31">
-        <v>3168</v>
-      </c>
-      <c r="D29" s="31" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="B30" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" s="31">
-        <v>2199</v>
-      </c>
-      <c r="D30" s="31" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="C31" s="31">
-        <v>4060</v>
-      </c>
-      <c r="D31" s="31" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" s="31">
-        <v>2819</v>
-      </c>
-      <c r="D32" s="31" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="C33" s="31">
-        <v>33822</v>
-      </c>
-      <c r="D33" s="31" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="B34" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="C34" s="31">
-        <v>40861</v>
-      </c>
-      <c r="D34" s="31" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="B35" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="C35" s="31">
-        <v>12046</v>
-      </c>
-      <c r="D35" s="31" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="B36" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="C36" s="31">
-        <v>4917</v>
-      </c>
-      <c r="D36" s="31" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="B37" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="C37" s="31">
-        <v>4121</v>
-      </c>
-      <c r="D37" s="31" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="B38" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="C38" s="31">
-        <v>24980</v>
-      </c>
-      <c r="D38" s="31" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="30" t="s">
+      <c r="C59" s="31">
+        <v>1775</v>
+      </c>
+      <c r="D59" s="31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" s="31">
-        <v>8193</v>
-      </c>
-      <c r="D39" s="31" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="30" t="s">
+      <c r="B60" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C60" s="33">
+        <v>46555</v>
+      </c>
+      <c r="D60" s="33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="14" thickBot="1">
+      <c r="A61" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="C40" s="31">
-        <v>0</v>
-      </c>
-      <c r="D40" s="31"/>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="B41" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="C41" s="31">
-        <v>4783</v>
-      </c>
-      <c r="D41" s="31" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="30" t="s">
+      <c r="B61" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="B42" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="C42" s="31">
-        <v>7492</v>
-      </c>
-      <c r="D42" s="31" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="B43" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C43" s="33">
-        <v>41280</v>
-      </c>
-      <c r="D43" s="33" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="B44" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="C44" s="33">
-        <v>11680</v>
-      </c>
-      <c r="D44" s="33" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="B45" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="C45" s="35">
-        <v>7522</v>
-      </c>
-      <c r="D45" s="35" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="B46" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="C46" s="35">
-        <v>6544</v>
-      </c>
-      <c r="D46" s="35" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="B47" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C47" s="35">
-        <v>14432</v>
-      </c>
-      <c r="D47" s="35" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="B48" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="C48" s="35">
-        <v>5161</v>
-      </c>
-      <c r="D48" s="35" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="B49" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="C49" s="35">
-        <v>11239</v>
-      </c>
-      <c r="D49" s="35" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="B50" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C50" s="37">
-        <v>2667</v>
-      </c>
-      <c r="D50" s="37" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B51" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C51" s="37">
-        <v>0</v>
-      </c>
-      <c r="D51" s="37"/>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="B52" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C52" s="37">
-        <v>3111</v>
-      </c>
-      <c r="D52" s="37" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="B53" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C53" s="37">
-        <v>1988</v>
-      </c>
-      <c r="D53" s="37" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="B54" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C54" s="37">
-        <v>5217</v>
-      </c>
-      <c r="D54" s="37" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="B55" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C55" s="37">
-        <v>2154</v>
-      </c>
-      <c r="D55" s="37" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="B56" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C56" s="37">
-        <v>1870</v>
-      </c>
-      <c r="D56" s="37" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="B57" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C57" s="37">
-        <v>7849</v>
-      </c>
-      <c r="D57" s="37" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="B58" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C58" s="37">
-        <v>3640</v>
-      </c>
-      <c r="D58" s="37" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="B59" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C59" s="37">
-        <v>1775</v>
-      </c>
-      <c r="D59" s="37" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="B60" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="C60" s="39">
-        <v>46555</v>
-      </c>
-      <c r="D60" s="39" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="14" thickBot="1">
-      <c r="A61" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="B61" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="C61" s="41">
+      <c r="C61" s="35">
         <v>35562</v>
       </c>
-      <c r="D61" s="41" t="s">
-        <v>16</v>
+      <c r="D61" s="35" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="42"/>
-      <c r="B62" s="43"/>
+      <c r="A62" s="36"/>
+      <c r="B62" s="37"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>